<commit_message>
1) Fixed the bug with in 'build_combined_dc_and_linearized_ac_opf_model' which prevents the power flow between transmission and distribution level.
2) Fragility data is moved from wcon to ncon, and specified for each network model in network_factory.py.

3) The investment_model.py is refined, and it is still under debugging.

4) Some small refinements around the project.
</commit_message>
<xml_diff>
--- a/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only.xlsx
+++ b/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\Manchester_Distribution_Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FC9A9E-2C50-46E2-8BDF-547A56420E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BF6A1D-C9D2-4F70-BC66-B3C9A682759A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_values" sheetId="1" r:id="rId1"/>
@@ -321,10 +321,6 @@
     <t>V_to (kV)</t>
   </si>
   <si>
-    <t xml:space="preserve">Type (1 for line, 0 for transformer)
-</t>
-  </si>
-  <si>
     <t>Length (km)</t>
   </si>
   <si>
@@ -455,6 +451,9 @@
   </si>
   <si>
     <t>gen_cost_coef_2</t>
+  </si>
+  <si>
+    <t>Type (1 for line, 0 for transformer)</t>
   </si>
 </sst>
 </file>
@@ -831,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47:D69"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3435,8 +3434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3470,25 +3469,25 @@
         <v>93</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
@@ -6625,7 +6624,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6645,28 +6644,28 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -6821,7 +6820,7 @@
         <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6">
         <v>15.817738160351359</v>
@@ -6857,7 +6856,7 @@
         <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7">
         <v>8.7183809790987699</v>
@@ -6893,7 +6892,7 @@
         <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8">
         <v>14.745301948651541</v>
@@ -6929,7 +6928,7 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9">
         <v>9.3392216532809886</v>
@@ -6965,7 +6964,7 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10">
         <v>10.66381232746668</v>
@@ -7001,7 +7000,7 @@
         <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11">
         <v>24.561448963248029</v>
@@ -7037,7 +7036,7 @@
         <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12">
         <v>17.18120772798412</v>
@@ -7073,7 +7072,7 @@
         <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13">
         <v>17.82439332308557</v>
@@ -7109,7 +7108,7 @@
         <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D14">
         <v>10.241879258445859</v>
@@ -7145,7 +7144,7 @@
         <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15">
         <v>6.0517216763918684</v>
@@ -7181,7 +7180,7 @@
         <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D16">
         <v>12.48369329419058</v>
@@ -7217,7 +7216,7 @@
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D17">
         <v>9.2036618442419424</v>
@@ -7253,7 +7252,7 @@
         <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D18">
         <v>11.25342699086633</v>
@@ -7289,7 +7288,7 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19">
         <v>13.51328567040467</v>
@@ -7325,7 +7324,7 @@
         <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D20">
         <v>12.471403817077681</v>
@@ -7361,7 +7360,7 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D21">
         <v>23.769442241105981</v>
@@ -7397,7 +7396,7 @@
         <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D22">
         <v>15.16358066810931</v>
@@ -7433,7 +7432,7 @@
         <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D23">
         <v>12.56492637502612</v>
@@ -7469,7 +7468,7 @@
         <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D24">
         <v>12.583011408930631</v>
@@ -7505,7 +7504,7 @@
         <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D25">
         <v>10.343775674877429</v>
@@ -7541,7 +7540,7 @@
         <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D26">
         <v>9.1184429123599724</v>
@@ -7577,7 +7576,7 @@
         <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27">
         <v>12.03819464418018</v>
@@ -7613,7 +7612,7 @@
         <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D28">
         <v>10.860025148287541</v>
@@ -7650,7 +7649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -7671,28 +7670,28 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -7819,7 +7818,7 @@
         <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6">
         <v>0.589363521</v>
@@ -7848,7 +7847,7 @@
         <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7">
         <v>1.8364710660000001</v>
@@ -7877,7 +7876,7 @@
         <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8">
         <v>0.80344782900000011</v>
@@ -7906,7 +7905,7 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9">
         <v>0.62217652800000001</v>
@@ -7935,7 +7934,7 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10">
         <v>1.547600925</v>
@@ -7964,7 +7963,7 @@
         <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11">
         <v>2.8933166199999998</v>
@@ -7993,7 +7992,7 @@
         <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E12">
         <v>5.3985405980000003</v>
@@ -8022,7 +8021,7 @@
         <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E13">
         <v>4.0841158010000003</v>
@@ -8051,7 +8050,7 @@
         <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14">
         <v>2.2803977</v>
@@ -8080,7 +8079,7 @@
         <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15">
         <v>1.0599167350000001</v>
@@ -8109,7 +8108,7 @@
         <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E16">
         <v>0.78897617400000009</v>
@@ -8138,7 +8137,7 @@
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E17">
         <v>1.0643096480000001</v>
@@ -8167,7 +8166,7 @@
         <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E18">
         <v>1.2779157539999999</v>
@@ -8196,7 +8195,7 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E19">
         <v>1.3368229119999999</v>
@@ -8225,7 +8224,7 @@
         <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20">
         <v>2.1107605889999999</v>
@@ -8254,7 +8253,7 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E21">
         <v>2.7248101920000001</v>
@@ -8283,7 +8282,7 @@
         <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E22">
         <v>0.71056749699999999</v>
@@ -8312,7 +8311,7 @@
         <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E23">
         <v>1.6215263440000001</v>
@@ -8341,7 +8340,7 @@
         <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E24">
         <v>0.63048667299999994</v>
@@ -8370,7 +8369,7 @@
         <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E25">
         <v>3.823861333</v>
@@ -8399,7 +8398,7 @@
         <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E26">
         <v>13.080431398</v>
@@ -8428,7 +8427,7 @@
         <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E27">
         <v>1.116071569</v>
@@ -8457,7 +8456,7 @@
         <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E28">
         <v>1.7886984909999999</v>

</xml_diff>

<commit_message>
1) Fixed the bug related to investment_model.py. Now 'build_investment_model' can run without error, but the model cannot be solved (i.e., the model is infeasible or unbounded). The next step is to debug the investment model.
</commit_message>
<xml_diff>
--- a/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only.xlsx
+++ b/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\Manchester_Distribution_Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BF6A1D-C9D2-4F70-BC66-B3C9A682759A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6178C21F-E5BA-4418-9418-E1919A537C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3435,7 +3435,7 @@
   <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3860,6 +3860,9 @@
       <c r="G10">
         <v>0</v>
       </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
       <c r="I10">
         <v>1.0395E-2</v>
       </c>
@@ -3895,6 +3898,9 @@
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
       <c r="I11">
         <v>1.0626E-2</v>
       </c>
@@ -3930,6 +3936,9 @@
       <c r="G12">
         <v>0</v>
       </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
       <c r="I12">
         <v>7.7340000000000004E-3</v>
       </c>
@@ -3965,6 +3974,9 @@
       <c r="G13">
         <v>0</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
       <c r="I13">
         <v>7.8269999999999989E-3</v>
       </c>
@@ -4000,6 +4012,9 @@
       <c r="G14">
         <v>0</v>
       </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
       <c r="I14">
         <v>5.6910000000000007E-3</v>
       </c>
@@ -4035,6 +4050,9 @@
       <c r="G15">
         <v>0</v>
       </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
       <c r="I15">
         <v>5.6910000000000007E-3</v>
       </c>
@@ -4070,6 +4088,9 @@
       <c r="G16">
         <v>0</v>
       </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
       <c r="I16">
         <v>8.1849999999999996E-3</v>
       </c>
@@ -4105,6 +4126,9 @@
       <c r="G17">
         <v>0</v>
       </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
       <c r="I17">
         <v>8.2959999999999996E-3</v>
       </c>
@@ -5516,6 +5540,9 @@
       <c r="G50">
         <v>0</v>
       </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
       <c r="I50">
         <v>1.985E-2</v>
       </c>
@@ -5551,6 +5578,9 @@
       <c r="G51">
         <v>0</v>
       </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
       <c r="I51">
         <v>0.02</v>
       </c>
@@ -5586,6 +5616,9 @@
       <c r="G52">
         <v>0</v>
       </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
       <c r="I52">
         <v>0.02</v>
       </c>
@@ -5621,6 +5654,9 @@
       <c r="G53">
         <v>0</v>
       </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
       <c r="I53">
         <v>0.02</v>
       </c>
@@ -5656,6 +5692,9 @@
       <c r="G54">
         <v>0</v>
       </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
       <c r="I54">
         <v>0.02</v>
       </c>
@@ -5691,6 +5730,9 @@
       <c r="G55">
         <v>0</v>
       </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
       <c r="I55">
         <v>0.02</v>
       </c>
@@ -5726,6 +5768,9 @@
       <c r="G56">
         <v>0</v>
       </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
       <c r="I56">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -5761,6 +5806,9 @@
       <c r="G57">
         <v>0</v>
       </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
       <c r="I57">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -5796,6 +5844,9 @@
       <c r="G58">
         <v>0</v>
       </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
       <c r="I58">
         <v>0.02</v>
       </c>
@@ -5831,6 +5882,9 @@
       <c r="G59">
         <v>0</v>
       </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
       <c r="I59">
         <v>0.02</v>
       </c>
@@ -5866,6 +5920,9 @@
       <c r="G60">
         <v>0</v>
       </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
       <c r="I60">
         <v>0.02</v>
       </c>
@@ -5901,6 +5958,9 @@
       <c r="G61">
         <v>0</v>
       </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
       <c r="I61">
         <v>0.02</v>
       </c>
@@ -5936,6 +5996,9 @@
       <c r="G62">
         <v>0</v>
       </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
       <c r="I62">
         <v>4.4299999999999999E-2</v>
       </c>
@@ -5971,6 +6034,9 @@
       <c r="G63">
         <v>0</v>
       </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
       <c r="I63">
         <v>0.02</v>
       </c>
@@ -6006,6 +6072,9 @@
       <c r="G64">
         <v>0</v>
       </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
       <c r="I64">
         <v>0.02</v>
       </c>
@@ -6041,6 +6110,9 @@
       <c r="G65">
         <v>0</v>
       </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
       <c r="I65">
         <v>0.02</v>
       </c>
@@ -6076,6 +6148,9 @@
       <c r="G66">
         <v>0</v>
       </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
       <c r="I66">
         <v>0.02</v>
       </c>
@@ -6111,6 +6186,9 @@
       <c r="G67">
         <v>0</v>
       </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
       <c r="I67">
         <v>0.02</v>
       </c>
@@ -6146,6 +6224,9 @@
       <c r="G68">
         <v>0</v>
       </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
       <c r="I68">
         <v>0.02</v>
       </c>
@@ -6179,6 +6260,9 @@
         <v>6.6</v>
       </c>
       <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
         <v>0</v>
       </c>
       <c r="I69">
@@ -6216,6 +6300,9 @@
       <c r="G70">
         <v>0</v>
       </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
       <c r="I70">
         <v>0.02</v>
       </c>
@@ -6251,6 +6338,9 @@
       <c r="G71">
         <v>0</v>
       </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
       <c r="I71">
         <v>0.02</v>
       </c>
@@ -6286,6 +6376,9 @@
       <c r="G72">
         <v>0</v>
       </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
       <c r="I72">
         <v>0.02</v>
       </c>
@@ -6321,6 +6414,9 @@
       <c r="G73">
         <v>0</v>
       </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
       <c r="I73">
         <v>0.02</v>
       </c>
@@ -6356,6 +6452,9 @@
       <c r="G74">
         <v>0</v>
       </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
       <c r="I74">
         <v>0.02</v>
       </c>
@@ -6391,6 +6490,9 @@
       <c r="G75">
         <v>0</v>
       </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
       <c r="I75">
         <v>0.02</v>
       </c>
@@ -6426,6 +6528,9 @@
       <c r="G76">
         <v>0</v>
       </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
       <c r="I76">
         <v>0.02</v>
       </c>
@@ -6461,6 +6566,9 @@
       <c r="G77">
         <v>0</v>
       </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
       <c r="I77">
         <v>0.02</v>
       </c>
@@ -6496,6 +6604,9 @@
       <c r="G78">
         <v>0</v>
       </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
       <c r="I78">
         <v>0.02</v>
       </c>
@@ -6531,6 +6642,9 @@
       <c r="G79">
         <v>0</v>
       </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
       <c r="I79">
         <v>0.02</v>
       </c>
@@ -6566,6 +6680,9 @@
       <c r="G80">
         <v>0</v>
       </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
       <c r="I80">
         <v>0.02</v>
       </c>
@@ -6599,6 +6716,9 @@
         <v>11</v>
       </c>
       <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
         <v>0</v>
       </c>
       <c r="I81">

</xml_diff>

<commit_message>
1) Added GB_Transmission_Network_29_Bus.xlsx which stores network data of a simplified (29-bus) GB transmission network. Currently the geo data (i.e., lons and lats) are manually assigned and do not reflect the real network topology.
2) Added  network models 'GB_Transmission_Network_29_Bus' and '29_bus_GB_transmission_network_with_kearsley_GSP_group' in network_factory.py. The networks can pass the corresponding power flow models in network.py.

3) Fixed an issue with the DC power flow model that the power flow values should be multiplied by the base_MVA value.
</commit_message>
<xml_diff>
--- a/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only.xlsx
+++ b/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\Manchester_Distribution_Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6178C21F-E5BA-4418-9418-E1919A537C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB4EC90-ADF4-4567-9282-6773F5A48FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_values" sheetId="1" r:id="rId1"/>
@@ -72,12 +72,6 @@
     <t>V_max (pu)</t>
   </si>
   <si>
-    <t>V_angle_min</t>
-  </si>
-  <si>
-    <t>V_angle_max</t>
-  </si>
-  <si>
     <t>Geo_lon</t>
   </si>
   <si>
@@ -333,12 +327,6 @@
     <t>Thermal Rating (Amp)</t>
   </si>
   <si>
-    <t>S_max</t>
-  </si>
-  <si>
-    <t>P_max</t>
-  </si>
-  <si>
     <t>DFES Name</t>
   </si>
   <si>
@@ -450,10 +438,22 @@
     <t>gen_cost_coef_1</t>
   </si>
   <si>
-    <t>gen_cost_coef_2</t>
-  </si>
-  <si>
     <t>Type (1 for line, 0 for transformer)</t>
+  </si>
+  <si>
+    <t>gen_cost_coef_0</t>
+  </si>
+  <si>
+    <t>S_max (MW)</t>
+  </si>
+  <si>
+    <t>P_max (MW)</t>
+  </si>
+  <si>
+    <t>V_angle_min (rad)</t>
+  </si>
+  <si>
+    <t>V_angle_max (rad)</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,6 +483,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -831,7 +837,7 @@
   <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:XFD63"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -839,7 +845,10 @@
     <col min="2" max="3" width="12.59765625" customWidth="1"/>
     <col min="4" max="4" width="21.53125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1328125" customWidth="1"/>
-    <col min="6" max="12" width="13.59765625" customWidth="1"/>
+    <col min="6" max="8" width="13.59765625" customWidth="1"/>
+    <col min="9" max="9" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -868,16 +877,16 @@
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
@@ -885,10 +894,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -920,10 +929,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -955,10 +964,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -990,10 +999,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1025,10 +1034,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1060,10 +1069,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1095,10 +1104,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1130,10 +1139,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1165,10 +1174,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1200,10 +1209,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1235,10 +1244,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1270,10 +1279,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1305,10 +1314,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1340,13 +1349,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1378,13 +1387,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
         <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>31</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1416,13 +1425,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1454,13 +1463,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1492,13 +1501,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1530,13 +1539,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1568,13 +1577,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1606,13 +1615,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
         <v>36</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1644,13 +1653,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1682,13 +1691,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1720,13 +1729,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1758,13 +1767,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1796,13 +1805,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1834,13 +1843,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1872,13 +1881,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
         <v>44</v>
-      </c>
-      <c r="D29" t="s">
-        <v>46</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1910,13 +1919,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1948,13 +1957,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1986,13 +1995,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -2024,13 +2033,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -2062,13 +2071,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -2100,13 +2109,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2138,13 +2147,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -2176,13 +2185,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -2214,13 +2223,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -2252,13 +2261,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2290,13 +2299,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -2328,13 +2337,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
         <v>57</v>
-      </c>
-      <c r="D41" t="s">
-        <v>59</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -2366,13 +2375,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2404,13 +2413,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -2442,13 +2451,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2480,13 +2489,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -2518,13 +2527,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2556,13 +2565,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -2594,13 +2603,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2632,13 +2641,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D49" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -2670,13 +2679,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2708,13 +2717,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2746,13 +2755,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -2784,13 +2793,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D53" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -2822,13 +2831,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -2860,13 +2869,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -2898,13 +2907,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D56" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -2936,13 +2945,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D57" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -2974,13 +2983,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -3012,13 +3021,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D59" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -3050,13 +3059,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D60" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -3088,13 +3097,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D61" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -3126,13 +3135,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D62" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -3164,13 +3173,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D63" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -3202,13 +3211,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D64" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -3240,13 +3249,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D65" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -3278,13 +3287,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D66" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -3316,13 +3325,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D67" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -3354,13 +3363,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C68" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D68" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -3392,13 +3401,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D69" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -3434,8 +3443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3446,48 +3455,48 @@
     <col min="4" max="4" width="21.9296875" bestFit="1" customWidth="1"/>
     <col min="5" max="10" width="13.59765625" customWidth="1"/>
     <col min="11" max="11" width="18.59765625" customWidth="1"/>
-    <col min="12" max="13" width="10.59765625" customWidth="1"/>
+    <col min="12" max="13" width="12.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
@@ -3495,13 +3504,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>132</v>
@@ -3538,13 +3547,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>132</v>
@@ -3581,13 +3590,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>132</v>
@@ -3624,13 +3633,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>132</v>
@@ -3667,13 +3676,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>132</v>
@@ -3710,13 +3719,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>132</v>
@@ -3753,13 +3762,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>132</v>
@@ -3798,13 +3807,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>132</v>
@@ -3843,13 +3852,13 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10">
         <v>132</v>
@@ -3881,13 +3890,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>132</v>
@@ -3919,13 +3928,13 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12">
         <v>132</v>
@@ -3957,13 +3966,13 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13">
         <v>132</v>
@@ -3995,13 +4004,13 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E14">
         <v>132</v>
@@ -4033,13 +4042,13 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E15">
         <v>132</v>
@@ -4071,13 +4080,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16">
         <v>132</v>
@@ -4109,13 +4118,13 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E17">
         <v>132</v>
@@ -4147,13 +4156,13 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18">
         <v>33</v>
@@ -4190,13 +4199,13 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19">
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19">
         <v>33</v>
@@ -4233,13 +4242,13 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>33</v>
@@ -4276,13 +4285,13 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E21">
         <v>33</v>
@@ -4319,13 +4328,13 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E22">
         <v>33</v>
@@ -4362,13 +4371,13 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E23">
         <v>33</v>
@@ -4405,13 +4414,13 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E24">
         <v>33</v>
@@ -4448,13 +4457,13 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E25">
         <v>33</v>
@@ -4491,13 +4500,13 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26">
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E26">
         <v>33</v>
@@ -4534,13 +4543,13 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27">
         <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27">
         <v>33</v>
@@ -4577,13 +4586,13 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C28">
         <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E28">
         <v>33</v>
@@ -4620,13 +4629,13 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C29">
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E29">
         <v>33</v>
@@ -4663,13 +4672,13 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C30">
         <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E30">
         <v>33</v>
@@ -4706,13 +4715,13 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C31">
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E31">
         <v>33</v>
@@ -4749,13 +4758,13 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C32">
         <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E32">
         <v>33</v>
@@ -4792,13 +4801,13 @@
         <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C33">
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E33">
         <v>33</v>
@@ -4835,13 +4844,13 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34">
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E34">
         <v>33</v>
@@ -4878,13 +4887,13 @@
         <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C35">
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E35">
         <v>33</v>
@@ -4921,13 +4930,13 @@
         <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C36">
         <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E36">
         <v>33</v>
@@ -4964,13 +4973,13 @@
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C37">
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E37">
         <v>33</v>
@@ -5007,13 +5016,13 @@
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C38">
         <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E38">
         <v>33</v>
@@ -5050,13 +5059,13 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C39">
         <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E39">
         <v>33</v>
@@ -5093,13 +5102,13 @@
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C40">
         <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E40">
         <v>33</v>
@@ -5136,13 +5145,13 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C41">
         <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E41">
         <v>33</v>
@@ -5179,13 +5188,13 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C42">
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E42">
         <v>33</v>
@@ -5222,13 +5231,13 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C43">
         <v>39</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E43">
         <v>33</v>
@@ -5265,13 +5274,13 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C44">
         <v>40</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E44">
         <v>33</v>
@@ -5308,13 +5317,13 @@
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C45">
         <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E45">
         <v>33</v>
@@ -5351,13 +5360,13 @@
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C46">
         <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E46">
         <v>33</v>
@@ -5394,13 +5403,13 @@
         <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C47">
         <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E47">
         <v>33</v>
@@ -5437,13 +5446,13 @@
         <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C48">
         <v>44</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E48">
         <v>33</v>
@@ -5480,13 +5489,13 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C49">
         <v>45</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E49">
         <v>33</v>
@@ -5523,13 +5532,13 @@
         <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C50">
         <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E50">
         <v>33</v>
@@ -5561,13 +5570,13 @@
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C51">
         <v>47</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E51">
         <v>33</v>
@@ -5599,13 +5608,13 @@
         <v>16</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52">
         <v>48</v>
       </c>
       <c r="D52" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E52">
         <v>33</v>
@@ -5637,13 +5646,13 @@
         <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C53">
         <v>49</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E53">
         <v>33</v>
@@ -5675,13 +5684,13 @@
         <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C54">
         <v>50</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E54">
         <v>33</v>
@@ -5713,13 +5722,13 @@
         <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C55">
         <v>50</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E55">
         <v>33</v>
@@ -5751,13 +5760,13 @@
         <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C56">
         <v>51</v>
       </c>
       <c r="D56" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E56">
         <v>33</v>
@@ -5789,13 +5798,13 @@
         <v>21</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C57">
         <v>51</v>
       </c>
       <c r="D57" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E57">
         <v>33</v>
@@ -5827,13 +5836,13 @@
         <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C58">
         <v>52</v>
       </c>
       <c r="D58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E58">
         <v>33</v>
@@ -5865,13 +5874,13 @@
         <v>23</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C59">
         <v>53</v>
       </c>
       <c r="D59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E59">
         <v>33</v>
@@ -5903,13 +5912,13 @@
         <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C60">
         <v>54</v>
       </c>
       <c r="D60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E60">
         <v>33</v>
@@ -5941,13 +5950,13 @@
         <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C61">
         <v>54</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E61">
         <v>33</v>
@@ -5979,13 +5988,13 @@
         <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C62">
         <v>55</v>
       </c>
       <c r="D62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E62">
         <v>33</v>
@@ -6017,13 +6026,13 @@
         <v>27</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C63">
         <v>56</v>
       </c>
       <c r="D63" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E63">
         <v>33</v>
@@ -6055,13 +6064,13 @@
         <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C64">
         <v>57</v>
       </c>
       <c r="D64" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E64">
         <v>33</v>
@@ -6093,13 +6102,13 @@
         <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C65">
         <v>57</v>
       </c>
       <c r="D65" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E65">
         <v>33</v>
@@ -6131,13 +6140,13 @@
         <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C66">
         <v>58</v>
       </c>
       <c r="D66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E66">
         <v>33</v>
@@ -6169,13 +6178,13 @@
         <v>31</v>
       </c>
       <c r="B67" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C67">
         <v>59</v>
       </c>
       <c r="D67" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E67">
         <v>33</v>
@@ -6207,13 +6216,13 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C68">
         <v>60</v>
       </c>
       <c r="D68" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E68">
         <v>33</v>
@@ -6245,13 +6254,13 @@
         <v>33</v>
       </c>
       <c r="B69" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C69">
         <v>61</v>
       </c>
       <c r="D69" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E69">
         <v>33</v>
@@ -6283,13 +6292,13 @@
         <v>34</v>
       </c>
       <c r="B70" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C70">
         <v>61</v>
       </c>
       <c r="D70" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E70">
         <v>33</v>
@@ -6321,13 +6330,13 @@
         <v>35</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C71">
         <v>62</v>
       </c>
       <c r="D71" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E71">
         <v>33</v>
@@ -6359,13 +6368,13 @@
         <v>36</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C72">
         <v>62</v>
       </c>
       <c r="D72" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E72">
         <v>33</v>
@@ -6397,13 +6406,13 @@
         <v>37</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C73">
         <v>63</v>
       </c>
       <c r="D73" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E73">
         <v>33</v>
@@ -6435,13 +6444,13 @@
         <v>38</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C74">
         <v>63</v>
       </c>
       <c r="D74" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E74">
         <v>33</v>
@@ -6473,13 +6482,13 @@
         <v>39</v>
       </c>
       <c r="B75" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C75">
         <v>64</v>
       </c>
       <c r="D75" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E75">
         <v>33</v>
@@ -6511,13 +6520,13 @@
         <v>40</v>
       </c>
       <c r="B76" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C76">
         <v>64</v>
       </c>
       <c r="D76" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E76">
         <v>33</v>
@@ -6549,13 +6558,13 @@
         <v>41</v>
       </c>
       <c r="B77" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C77">
         <v>65</v>
       </c>
       <c r="D77" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E77">
         <v>33</v>
@@ -6587,13 +6596,13 @@
         <v>42</v>
       </c>
       <c r="B78" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C78">
         <v>66</v>
       </c>
       <c r="D78" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E78">
         <v>33</v>
@@ -6625,13 +6634,13 @@
         <v>43</v>
       </c>
       <c r="B79" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C79">
         <v>67</v>
       </c>
       <c r="D79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E79">
         <v>33</v>
@@ -6663,13 +6672,13 @@
         <v>44</v>
       </c>
       <c r="B80" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C80">
         <v>68</v>
       </c>
       <c r="D80" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E80">
         <v>33</v>
@@ -6701,13 +6710,13 @@
         <v>45</v>
       </c>
       <c r="B81" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C81">
         <v>68</v>
       </c>
       <c r="D81" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E81">
         <v>33</v>
@@ -6744,7 +6753,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6764,28 +6773,28 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -6793,10 +6802,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>62.990131895094009</v>
@@ -6829,10 +6838,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>80.871689211959065</v>
@@ -6865,10 +6874,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>100.87403825175321</v>
@@ -6901,10 +6910,10 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>70.824781345557497</v>
@@ -6937,10 +6946,10 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D6">
         <v>15.817738160351359</v>
@@ -6973,10 +6982,10 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <v>8.7183809790987699</v>
@@ -7009,10 +7018,10 @@
         <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D8">
         <v>14.745301948651541</v>
@@ -7045,10 +7054,10 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D9">
         <v>9.3392216532809886</v>
@@ -7081,10 +7090,10 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D10">
         <v>10.66381232746668</v>
@@ -7117,10 +7126,10 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D11">
         <v>24.561448963248029</v>
@@ -7153,10 +7162,10 @@
         <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D12">
         <v>17.18120772798412</v>
@@ -7189,10 +7198,10 @@
         <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D13">
         <v>17.82439332308557</v>
@@ -7225,10 +7234,10 @@
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D14">
         <v>10.241879258445859</v>
@@ -7261,10 +7270,10 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D15">
         <v>6.0517216763918684</v>
@@ -7297,10 +7306,10 @@
         <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D16">
         <v>12.48369329419058</v>
@@ -7333,10 +7342,10 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D17">
         <v>9.2036618442419424</v>
@@ -7369,10 +7378,10 @@
         <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D18">
         <v>11.25342699086633</v>
@@ -7405,10 +7414,10 @@
         <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D19">
         <v>13.51328567040467</v>
@@ -7441,10 +7450,10 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D20">
         <v>12.471403817077681</v>
@@ -7477,10 +7486,10 @@
         <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D21">
         <v>23.769442241105981</v>
@@ -7513,10 +7522,10 @@
         <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D22">
         <v>15.16358066810931</v>
@@ -7549,10 +7558,10 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D23">
         <v>12.56492637502612</v>
@@ -7585,10 +7594,10 @@
         <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D24">
         <v>12.583011408930631</v>
@@ -7621,10 +7630,10 @@
         <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D25">
         <v>10.343775674877429</v>
@@ -7657,10 +7666,10 @@
         <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D26">
         <v>9.1184429123599724</v>
@@ -7693,10 +7702,10 @@
         <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D27">
         <v>12.03819464418018</v>
@@ -7729,10 +7738,10 @@
         <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D28">
         <v>10.860025148287541</v>
@@ -7769,8 +7778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7790,28 +7799,28 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -7819,10 +7828,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>3.5625888020000001</v>
@@ -7848,10 +7857,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>15.716287454</v>
@@ -7877,10 +7886,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4">
         <v>11.635689107999999</v>
@@ -7906,10 +7915,10 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>58.798036150999998</v>
@@ -7935,10 +7944,10 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E6">
         <v>0.589363521</v>
@@ -7964,10 +7973,10 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E7">
         <v>1.8364710660000001</v>
@@ -7993,10 +8002,10 @@
         <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E8">
         <v>0.80344782900000011</v>
@@ -8022,10 +8031,10 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E9">
         <v>0.62217652800000001</v>
@@ -8051,10 +8060,10 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E10">
         <v>1.547600925</v>
@@ -8080,10 +8089,10 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E11">
         <v>2.8933166199999998</v>
@@ -8109,10 +8118,10 @@
         <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E12">
         <v>5.3985405980000003</v>
@@ -8138,10 +8147,10 @@
         <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E13">
         <v>4.0841158010000003</v>
@@ -8167,10 +8176,10 @@
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E14">
         <v>2.2803977</v>
@@ -8196,10 +8205,10 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E15">
         <v>1.0599167350000001</v>
@@ -8225,10 +8234,10 @@
         <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E16">
         <v>0.78897617400000009</v>
@@ -8254,10 +8263,10 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E17">
         <v>1.0643096480000001</v>
@@ -8283,10 +8292,10 @@
         <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E18">
         <v>1.2779157539999999</v>
@@ -8312,10 +8321,10 @@
         <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E19">
         <v>1.3368229119999999</v>
@@ -8341,10 +8350,10 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E20">
         <v>2.1107605889999999</v>
@@ -8370,10 +8379,10 @@
         <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E21">
         <v>2.7248101920000001</v>
@@ -8399,10 +8408,10 @@
         <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E22">
         <v>0.71056749699999999</v>
@@ -8428,10 +8437,10 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E23">
         <v>1.6215263440000001</v>
@@ -8457,10 +8466,10 @@
         <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E24">
         <v>0.63048667299999994</v>
@@ -8486,10 +8495,10 @@
         <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E25">
         <v>3.823861333</v>
@@ -8515,10 +8524,10 @@
         <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E26">
         <v>13.080431398</v>
@@ -8544,10 +8553,10 @@
         <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E27">
         <v>1.116071569</v>
@@ -8573,10 +8582,10 @@
         <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E28">
         <v>1.7886984909999999</v>
@@ -8598,6 +8607,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1) Fixed the bug that line_hrdn values are always zero.
2) Added a data field 'bch_hardenable' that read from the column "If Hardenable" in the network model .xlsx files. Now it can be pre-defined that if a line is hardenable. Now the model can be solved with a 5 windstorm-scenario case.
</commit_message>
<xml_diff>
--- a/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only.xlsx
+++ b/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\Manchester_Distribution_Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB4EC90-ADF4-4567-9282-6773F5A48FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7DCAEB-13E8-4F03-8CA6-82B14C680A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_values" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="140">
   <si>
     <t>Name</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>V_angle_max (rad)</t>
+  </si>
+  <si>
+    <t>If Hardenable</t>
   </si>
 </sst>
 </file>
@@ -837,7 +840,7 @@
   <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="K2" sqref="K2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3441,10 +3444,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3453,12 +3456,12 @@
     <col min="2" max="2" width="20.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.59765625" customWidth="1"/>
     <col min="4" max="4" width="21.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="13.59765625" customWidth="1"/>
-    <col min="11" max="11" width="18.59765625" customWidth="1"/>
-    <col min="12" max="13" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="13.59765625" customWidth="1"/>
+    <col min="12" max="12" width="18.59765625" customWidth="1"/>
+    <col min="13" max="14" width="12.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -3480,26 +3483,29 @@
       <c r="G1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3522,27 +3528,30 @@
         <v>1</v>
       </c>
       <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>6.2060000000000004</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>4.0321549999999999E-3</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>9.7586500000000007E-3</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>573</v>
       </c>
-      <c r="L2">
-        <f t="shared" ref="L2:L9" si="0">SQRT(3)*E2*K2/1000</f>
+      <c r="M2">
+        <f t="shared" ref="M2:M9" si="0">SQRT(3)*E2*L2/1000</f>
         <v>131.00539488127959</v>
       </c>
-      <c r="M2">
-        <f t="shared" ref="M2:M9" si="1">L2</f>
+      <c r="N2">
+        <f t="shared" ref="N2:N9" si="1">M2</f>
         <v>131.00539488127959</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3565,27 +3574,30 @@
         <v>1</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>7.0419999999999998</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5.1057120000000001E-3</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>1.3585633999999999E-2</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>573</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f t="shared" si="0"/>
         <v>131.00539488127959</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <f t="shared" si="1"/>
         <v>131.00539488127959</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3608,27 +3620,30 @@
         <v>1</v>
       </c>
       <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>13.63</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>3.46E-3</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2.657E-2</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>815</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f t="shared" si="0"/>
         <v>186.33402587825981</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <f t="shared" si="1"/>
         <v>186.33402587825981</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3651,27 +3666,30 @@
         <v>1</v>
       </c>
       <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>13.63</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>3.5699999999999998E-3</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2.5360000000000001E-2</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>815</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f t="shared" si="0"/>
         <v>186.33402587825981</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <f t="shared" si="1"/>
         <v>186.33402587825981</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3694,27 +3712,30 @@
         <v>1</v>
       </c>
       <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>10.34</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>3.6679999999999998E-3</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1.7755679999999999E-2</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>866</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f t="shared" si="0"/>
         <v>197.99419191481348</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <f t="shared" si="1"/>
         <v>197.99419191481348</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3737,27 +3758,30 @@
         <v>1</v>
       </c>
       <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
         <v>10.28</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>3.659550000000001E-3</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1.7808359999999999E-2</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>866</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="0"/>
         <v>197.99419191481348</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f t="shared" si="1"/>
         <v>197.99419191481348</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3780,29 +3804,32 @@
         <v>1</v>
       </c>
       <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>8.36</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>3.5147199999999998E-3</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1.7610210000000001E-2</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>428.63883621654043</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="0"/>
         <v>98.000000000000014</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f t="shared" si="1"/>
         <v>98.000000000000014</v>
       </c>
-      <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3825,29 +3852,32 @@
         <v>1</v>
       </c>
       <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>8.51</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>3.5957200000000002E-3</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1.780021E-2</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>428.63883621654043</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="0"/>
         <v>98.000000000000014</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f t="shared" si="1"/>
         <v>98.000000000000014</v>
       </c>
-      <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3873,19 +3903,22 @@
         <v>0</v>
       </c>
       <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>1.0395E-2</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.28947341773468599</v>
-      </c>
-      <c r="L10">
-        <v>60</v>
       </c>
       <c r="M10">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="N10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>3</v>
       </c>
@@ -3911,19 +3944,22 @@
         <v>0</v>
       </c>
       <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>1.0626E-2</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.28846435433862527</v>
-      </c>
-      <c r="L11">
-        <v>60</v>
       </c>
       <c r="M11">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="N11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>4</v>
       </c>
@@ -3949,19 +3985,22 @@
         <v>0</v>
       </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>7.7340000000000004E-3</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.23264147984398659</v>
-      </c>
-      <c r="L12">
-        <v>90</v>
       </c>
       <c r="M12">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="N12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>5</v>
       </c>
@@ -3987,19 +4026,22 @@
         <v>0</v>
       </c>
       <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
         <v>7.8269999999999989E-3</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.23208805757944551</v>
-      </c>
-      <c r="L13">
-        <v>90</v>
       </c>
       <c r="M13">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="N13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>6</v>
       </c>
@@ -4025,19 +4067,22 @@
         <v>0</v>
       </c>
       <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
         <v>5.6910000000000007E-3</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.28000000000000003</v>
-      </c>
-      <c r="L14">
-        <v>90</v>
       </c>
       <c r="M14">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="N14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>7</v>
       </c>
@@ -4063,19 +4108,22 @@
         <v>0</v>
       </c>
       <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
         <v>5.6910000000000007E-3</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>0.28000000000000003</v>
-      </c>
-      <c r="L15">
-        <v>90</v>
       </c>
       <c r="M15">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="N15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>8</v>
       </c>
@@ -4101,19 +4149,22 @@
         <v>0</v>
       </c>
       <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
         <v>8.1849999999999996E-3</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>0.25319773828966169</v>
-      </c>
-      <c r="L16">
-        <v>90</v>
       </c>
       <c r="M16">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9</v>
       </c>
@@ -4139,19 +4190,22 @@
         <v>0</v>
       </c>
       <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
         <v>8.2959999999999996E-3</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>0.25097292380653341</v>
-      </c>
-      <c r="L17">
-        <v>90</v>
       </c>
       <c r="M17">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N17">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>10</v>
       </c>
@@ -4174,27 +4228,30 @@
         <v>1</v>
       </c>
       <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <v>5.7843499999999999</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>5.4777800000000001E-2</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>4.7662999999999997E-2</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>310</v>
       </c>
-      <c r="L18">
-        <f t="shared" ref="L18:L49" si="2">SQRT(3)*E18*K18/1000</f>
+      <c r="M18">
+        <f t="shared" ref="M18:M49" si="2">SQRT(3)*E18*L18/1000</f>
         <v>17.718879761429612</v>
       </c>
-      <c r="M18">
-        <f t="shared" ref="M18:M49" si="3">L18</f>
+      <c r="N18">
+        <f t="shared" ref="N18:N49" si="3">M18</f>
         <v>17.718879761429612</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>10</v>
       </c>
@@ -4217,27 +4274,30 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="I19">
+        <v>0.95</v>
+      </c>
+      <c r="J19">
         <v>8.9960000000000005E-3</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>7.8279999999999999E-3</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>356</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <f t="shared" si="2"/>
         <v>20.348132887319167</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <f t="shared" si="3"/>
         <v>20.348132887319167</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>10</v>
       </c>
@@ -4260,27 +4320,30 @@
         <v>1</v>
       </c>
       <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>3.129238</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>1.9063179999999999E-2</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>2.8081160000000001E-2</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>435</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <f t="shared" si="2"/>
         <v>24.863589342651231</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <f t="shared" si="3"/>
         <v>24.863589342651231</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>10</v>
       </c>
@@ -4303,27 +4366,30 @@
         <v>1</v>
       </c>
       <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
         <v>3.5166789999999999</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>3.292254E-2</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>3.0852170000000002E-2</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>356</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <f t="shared" si="2"/>
         <v>20.348132887319167</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <f t="shared" si="3"/>
         <v>20.348132887319167</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>10</v>
       </c>
@@ -4346,27 +4412,30 @@
         <v>1</v>
       </c>
       <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
         <v>2.1812260000000001</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>3.0764199999999998E-2</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>1.948809E-2</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>250</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <f t="shared" si="2"/>
         <v>14.289419162443236</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <f t="shared" si="3"/>
         <v>14.289419162443236</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>10</v>
       </c>
@@ -4389,27 +4458,30 @@
         <v>1</v>
       </c>
       <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
         <v>2.1881520000000001</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>3.085214E-2</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>1.9548030000000001E-2</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>250</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <f t="shared" si="2"/>
         <v>14.289419162443236</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <f t="shared" si="3"/>
         <v>14.289419162443236</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>11</v>
       </c>
@@ -4432,27 +4504,30 @@
         <v>1</v>
       </c>
       <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
         <v>2.2576101</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>1.8363391E-2</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>1.6322571000000001E-2</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>476</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <f t="shared" si="2"/>
         <v>27.207054085291922</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <f t="shared" si="3"/>
         <v>27.207054085291922</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>11</v>
       </c>
@@ -4475,27 +4550,30 @@
         <v>1</v>
       </c>
       <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
         <v>2.5233300000000001</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>1.4829500000000001E-2</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>2.5256500000000001E-2</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>670</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <f t="shared" si="2"/>
         <v>38.29564335534787</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <f t="shared" si="3"/>
         <v>38.29564335534787</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>11</v>
       </c>
@@ -4518,27 +4596,30 @@
         <v>1</v>
       </c>
       <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
         <v>2.95519</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>2.7986E-2</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>2.4351000000000001E-2</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>400</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <f t="shared" si="2"/>
         <v>22.86307065990918</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <f t="shared" si="3"/>
         <v>22.86307065990918</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>11</v>
       </c>
@@ -4561,27 +4642,30 @@
         <v>1</v>
       </c>
       <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
         <v>4.2699999999999996</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>6.1243400000000003E-2</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>5.8050200000000003E-2</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>245</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <f t="shared" si="2"/>
         <v>14.003630779194371</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <f t="shared" si="3"/>
         <v>14.003630779194371</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>11</v>
       </c>
@@ -4604,27 +4688,30 @@
         <v>1</v>
       </c>
       <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
         <v>1.3246150000000001</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>1.826792E-2</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>1.196001E-2</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>245</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <f t="shared" si="2"/>
         <v>14.003630779194371</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <f t="shared" si="3"/>
         <v>14.003630779194371</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>11</v>
       </c>
@@ -4647,27 +4734,30 @@
         <v>1</v>
       </c>
       <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
         <v>1.3198372</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>1.3187098E-2</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>1.1876604000000001E-2</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>356</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <f t="shared" si="2"/>
         <v>20.348132887319167</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <f t="shared" si="3"/>
         <v>20.348132887319167</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>11</v>
       </c>
@@ -4690,27 +4780,30 @@
         <v>1</v>
       </c>
       <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
         <v>2.6663199999999998</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>2.3896000000000001E-2</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>2.8646999999999999E-2</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>362</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <f t="shared" si="2"/>
         <v>20.691078947217807</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <f t="shared" si="3"/>
         <v>20.691078947217807</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>12</v>
       </c>
@@ -4733,27 +4826,30 @@
         <v>1</v>
       </c>
       <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
         <v>5.0938220000000003</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>5.8381624999999999E-2</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>4.3529178000000002E-2</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>235</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <f t="shared" si="2"/>
         <v>13.432054012696643</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <f t="shared" si="3"/>
         <v>13.432054012696643</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>12</v>
       </c>
@@ -4776,27 +4872,30 @@
         <v>1</v>
       </c>
       <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
         <v>3</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>3.5142800000000002E-2</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>2.7158450000000001E-2</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>263</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <f t="shared" si="2"/>
         <v>15.032468958890284</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <f t="shared" si="3"/>
         <v>15.032468958890284</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>12</v>
       </c>
@@ -4819,27 +4918,30 @@
         <v>1</v>
       </c>
       <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
         <v>2.584381</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>2.002837E-2</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>1.8625470000000002E-2</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>476</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <f t="shared" si="2"/>
         <v>27.207054085291922</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <f t="shared" si="3"/>
         <v>27.207054085291922</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>12</v>
       </c>
@@ -4862,27 +4964,30 @@
         <v>1</v>
       </c>
       <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
         <v>5.0221600000000004</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>5.927607E-2</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>5.3170799999999997E-2</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>245</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <f t="shared" si="2"/>
         <v>14.003630779194371</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <f t="shared" si="3"/>
         <v>14.003630779194371</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>12</v>
       </c>
@@ -4905,27 +5010,30 @@
         <v>1</v>
       </c>
       <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
         <v>2.7840690000000001</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>1.9649920000000001E-2</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>1.9934520000000001E-2</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>245</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <f t="shared" si="2"/>
         <v>14.003630779194371</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <f t="shared" si="3"/>
         <v>14.003630779194371</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>12</v>
       </c>
@@ -4948,27 +5056,30 @@
         <v>1</v>
       </c>
       <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
         <v>3.1139999999999999</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>2.9671510000000002E-2</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>2.5923930000000001E-2</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>356</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <f t="shared" si="2"/>
         <v>20.348132887319167</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <f t="shared" si="3"/>
         <v>20.348132887319167</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>12</v>
       </c>
@@ -4991,27 +5102,30 @@
         <v>1</v>
       </c>
       <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
         <v>2.391</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>1.2504075E-2</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>2.260357E-2</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>356</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <f t="shared" si="2"/>
         <v>20.348132887319167</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <f t="shared" si="3"/>
         <v>20.348132887319167</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>12</v>
       </c>
@@ -5034,27 +5148,30 @@
         <v>1</v>
       </c>
       <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
         <v>2.5080035299999999</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>1.3104360000000001E-2</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>2.3718400000000001E-2</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>356</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <f t="shared" si="2"/>
         <v>20.348132887319167</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <f t="shared" si="3"/>
         <v>20.348132887319167</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>12</v>
       </c>
@@ -5077,27 +5194,30 @@
         <v>1</v>
       </c>
       <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
         <v>0.13800000000000001</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>1.4120000000000001E-3</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>1.2899999999999999E-3</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>356</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <f t="shared" si="2"/>
         <v>20.348132887319167</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <f t="shared" si="3"/>
         <v>20.348132887319167</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>12</v>
       </c>
@@ -5120,27 +5240,30 @@
         <v>1</v>
       </c>
       <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
         <v>0.14599999999999999</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>1.4940000000000001E-3</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>1.3649999999999999E-3</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>356</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <f t="shared" si="2"/>
         <v>20.348132887319167</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <f t="shared" si="3"/>
         <v>20.348132887319167</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>12</v>
       </c>
@@ -5163,27 +5286,30 @@
         <v>1</v>
       </c>
       <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
         <v>1.9339999999999999</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>1.389489E-2</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>1.387261E-2</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>400</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <f t="shared" si="2"/>
         <v>22.86307065990918</v>
       </c>
-      <c r="M41">
+      <c r="N41">
         <f t="shared" si="3"/>
         <v>22.86307065990918</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>12</v>
       </c>
@@ -5206,27 +5332,30 @@
         <v>1</v>
       </c>
       <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
         <v>3.4409999999999998</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>2.7682040000000002E-2</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>2.4859948E-2</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>400</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <f t="shared" si="2"/>
         <v>22.86307065990918</v>
       </c>
-      <c r="M42">
+      <c r="N42">
         <f t="shared" si="3"/>
         <v>22.86307065990918</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>13</v>
       </c>
@@ -5249,27 +5378,30 @@
         <v>1</v>
       </c>
       <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
         <v>2.1939579999999999</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>1.467422E-2</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>1.553006E-2</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>492</v>
       </c>
-      <c r="L43">
+      <c r="M43">
         <f t="shared" si="2"/>
         <v>28.121576911688287</v>
       </c>
-      <c r="M43">
+      <c r="N43">
         <f t="shared" si="3"/>
         <v>28.121576911688287</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>13</v>
       </c>
@@ -5292,27 +5424,30 @@
         <v>1</v>
       </c>
       <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
         <v>1.0510299999999999</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>8.3079999999999994E-3</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>9.1750000000000009E-3</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>400</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <f t="shared" si="2"/>
         <v>22.86307065990918</v>
       </c>
-      <c r="M44">
+      <c r="N44">
         <f t="shared" si="3"/>
         <v>22.86307065990918</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>13</v>
       </c>
@@ -5335,27 +5470,30 @@
         <v>1</v>
       </c>
       <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
         <v>3.7915239999999999</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>3.0043871999999999E-2</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>2.7329301E-2</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>476</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <f t="shared" si="2"/>
         <v>27.207054085291922</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <f t="shared" si="3"/>
         <v>27.207054085291922</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>13</v>
       </c>
@@ -5378,27 +5516,30 @@
         <v>1</v>
       </c>
       <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
         <v>3.36</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>2.2181124999999999E-2</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>2.869288E-2</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>502</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <f t="shared" si="2"/>
         <v>28.693153678186018</v>
       </c>
-      <c r="M46">
+      <c r="N46">
         <f t="shared" si="3"/>
         <v>28.693153678186018</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>13</v>
       </c>
@@ -5421,27 +5562,30 @@
         <v>1</v>
       </c>
       <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
         <v>6.3639999999999999</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>7.7113680000000004E-2</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>0.13051534000000001</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <v>356</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <f t="shared" si="2"/>
         <v>20.348132887319167</v>
       </c>
-      <c r="M47">
+      <c r="N47">
         <f t="shared" si="3"/>
         <v>20.348132887319167</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>13</v>
       </c>
@@ -5464,27 +5608,30 @@
         <v>1</v>
       </c>
       <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
         <v>1.939527</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>1.443473E-2</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>1.3882240000000001E-2</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>476</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <f t="shared" si="2"/>
         <v>27.207054085291922</v>
       </c>
-      <c r="M48">
+      <c r="N48">
         <f t="shared" si="3"/>
         <v>27.207054085291922</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>13</v>
       </c>
@@ -5507,27 +5654,30 @@
         <v>1</v>
       </c>
       <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
         <v>3.0897000000000001</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>1.6757770000000002E-2</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>1.5869830000000001E-2</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>476</v>
       </c>
-      <c r="L49">
+      <c r="M49">
         <f t="shared" si="2"/>
         <v>27.207054085291922</v>
       </c>
-      <c r="M49">
+      <c r="N49">
         <f t="shared" si="3"/>
         <v>27.207054085291922</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>14</v>
       </c>
@@ -5553,19 +5703,22 @@
         <v>0</v>
       </c>
       <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
         <v>1.985E-2</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>0.58260000000000001</v>
-      </c>
-      <c r="L50">
-        <v>23</v>
       </c>
       <c r="M50">
         <v>23</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N50">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>15</v>
       </c>
@@ -5591,19 +5744,22 @@
         <v>0</v>
       </c>
       <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
         <v>0.02</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>0.52</v>
-      </c>
-      <c r="L51">
-        <v>20</v>
       </c>
       <c r="M51">
         <v>20</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>16</v>
       </c>
@@ -5629,19 +5785,22 @@
         <v>0</v>
       </c>
       <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
         <v>0.02</v>
       </c>
-      <c r="J52">
-        <v>0.5</v>
-      </c>
-      <c r="L52">
-        <v>23</v>
+      <c r="K52">
+        <v>0.5</v>
       </c>
       <c r="M52">
         <v>23</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N52">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>17</v>
       </c>
@@ -5667,19 +5826,22 @@
         <v>0</v>
       </c>
       <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
         <v>0.02</v>
       </c>
-      <c r="J53">
-        <v>0.5</v>
-      </c>
-      <c r="L53">
-        <v>23</v>
+      <c r="K53">
+        <v>0.5</v>
       </c>
       <c r="M53">
         <v>23</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N53">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>18</v>
       </c>
@@ -5705,19 +5867,22 @@
         <v>0</v>
       </c>
       <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
         <v>0.02</v>
       </c>
-      <c r="J54">
-        <v>0.5</v>
-      </c>
-      <c r="L54">
-        <v>23</v>
+      <c r="K54">
+        <v>0.5</v>
       </c>
       <c r="M54">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N54">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>19</v>
       </c>
@@ -5743,19 +5908,22 @@
         <v>0</v>
       </c>
       <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
         <v>0.02</v>
       </c>
-      <c r="J55">
-        <v>0.5</v>
-      </c>
-      <c r="L55">
-        <v>23</v>
+      <c r="K55">
+        <v>0.5</v>
       </c>
       <c r="M55">
         <v>23</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N55">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>20</v>
       </c>
@@ -5781,19 +5949,22 @@
         <v>0</v>
       </c>
       <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>0.35</v>
-      </c>
-      <c r="L56">
-        <v>38</v>
       </c>
       <c r="M56">
         <v>38</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N56">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>21</v>
       </c>
@@ -5819,19 +5990,22 @@
         <v>0</v>
       </c>
       <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>0.35</v>
-      </c>
-      <c r="L57">
-        <v>38</v>
       </c>
       <c r="M57">
         <v>38</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N57">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>22</v>
       </c>
@@ -5857,19 +6031,22 @@
         <v>0</v>
       </c>
       <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
         <v>0.02</v>
       </c>
-      <c r="J58">
-        <v>0.5</v>
-      </c>
-      <c r="L58">
-        <v>23</v>
+      <c r="K58">
+        <v>0.5</v>
       </c>
       <c r="M58">
         <v>23</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N58">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>23</v>
       </c>
@@ -5895,19 +6072,22 @@
         <v>0</v>
       </c>
       <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
         <v>0.02</v>
       </c>
-      <c r="J59">
-        <v>0.5</v>
-      </c>
-      <c r="L59">
-        <v>28</v>
+      <c r="K59">
+        <v>0.5</v>
       </c>
       <c r="M59">
         <v>28</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N59">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>24</v>
       </c>
@@ -5933,19 +6113,22 @@
         <v>0</v>
       </c>
       <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
         <v>0.02</v>
       </c>
-      <c r="J60">
-        <v>0.5</v>
-      </c>
-      <c r="L60">
-        <v>28</v>
+      <c r="K60">
+        <v>0.5</v>
       </c>
       <c r="M60">
         <v>28</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N60">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>25</v>
       </c>
@@ -5971,19 +6154,22 @@
         <v>0</v>
       </c>
       <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
         <v>0.02</v>
       </c>
-      <c r="J61">
-        <v>0.5</v>
-      </c>
-      <c r="L61">
-        <v>28</v>
+      <c r="K61">
+        <v>0.5</v>
       </c>
       <c r="M61">
         <v>28</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N61">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>26</v>
       </c>
@@ -6009,19 +6195,22 @@
         <v>0</v>
       </c>
       <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
         <v>4.4299999999999999E-2</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>0.57600000000000007</v>
-      </c>
-      <c r="L62">
-        <v>23</v>
       </c>
       <c r="M62">
         <v>23</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>27</v>
       </c>
@@ -6047,19 +6236,22 @@
         <v>0</v>
       </c>
       <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
         <v>0.02</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>0.52</v>
-      </c>
-      <c r="L63">
-        <v>20</v>
       </c>
       <c r="M63">
         <v>20</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>28</v>
       </c>
@@ -6085,19 +6277,22 @@
         <v>0</v>
       </c>
       <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
         <v>0.02</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>0.52</v>
-      </c>
-      <c r="L64">
-        <v>30</v>
       </c>
       <c r="M64">
         <v>30</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N64">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>29</v>
       </c>
@@ -6123,19 +6318,22 @@
         <v>0</v>
       </c>
       <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
         <v>0.02</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>0.52</v>
-      </c>
-      <c r="L65">
-        <v>30</v>
       </c>
       <c r="M65">
         <v>30</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>30</v>
       </c>
@@ -6161,19 +6359,22 @@
         <v>0</v>
       </c>
       <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
         <v>0.02</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>0.52</v>
-      </c>
-      <c r="L66">
-        <v>28</v>
       </c>
       <c r="M66">
         <v>28</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N66">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>31</v>
       </c>
@@ -6199,19 +6400,22 @@
         <v>0</v>
       </c>
       <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
         <v>0.02</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>0.52</v>
-      </c>
-      <c r="L67">
-        <v>28</v>
       </c>
       <c r="M67">
         <v>28</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N67">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>32</v>
       </c>
@@ -6237,19 +6441,22 @@
         <v>0</v>
       </c>
       <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
         <v>0.02</v>
       </c>
-      <c r="J68">
-        <v>0.5</v>
-      </c>
-      <c r="L68">
-        <v>23</v>
+      <c r="K68">
+        <v>0.5</v>
       </c>
       <c r="M68">
         <v>23</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N68">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>33</v>
       </c>
@@ -6275,19 +6482,22 @@
         <v>0</v>
       </c>
       <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
         <v>0.02</v>
       </c>
-      <c r="J69">
-        <v>0.5</v>
-      </c>
-      <c r="L69">
-        <v>30</v>
+      <c r="K69">
+        <v>0.5</v>
       </c>
       <c r="M69">
         <v>30</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N69">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>34</v>
       </c>
@@ -6313,19 +6523,22 @@
         <v>0</v>
       </c>
       <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
         <v>0.02</v>
       </c>
-      <c r="J70">
-        <v>0.5</v>
-      </c>
-      <c r="L70">
-        <v>30</v>
+      <c r="K70">
+        <v>0.5</v>
       </c>
       <c r="M70">
         <v>30</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N70">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>35</v>
       </c>
@@ -6351,19 +6564,22 @@
         <v>0</v>
       </c>
       <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
         <v>0.02</v>
       </c>
-      <c r="J71">
-        <v>0.5</v>
-      </c>
-      <c r="L71">
-        <v>23</v>
+      <c r="K71">
+        <v>0.5</v>
       </c>
       <c r="M71">
         <v>23</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N71">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>36</v>
       </c>
@@ -6389,19 +6605,22 @@
         <v>0</v>
       </c>
       <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
         <v>0.02</v>
       </c>
-      <c r="J72">
-        <v>0.5</v>
-      </c>
-      <c r="L72">
-        <v>23</v>
+      <c r="K72">
+        <v>0.5</v>
       </c>
       <c r="M72">
         <v>23</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N72">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>37</v>
       </c>
@@ -6427,19 +6646,22 @@
         <v>0</v>
       </c>
       <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
         <v>0.02</v>
       </c>
-      <c r="J73">
-        <v>0.5</v>
-      </c>
-      <c r="L73">
-        <v>23</v>
+      <c r="K73">
+        <v>0.5</v>
       </c>
       <c r="M73">
         <v>23</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N73">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>38</v>
       </c>
@@ -6465,19 +6687,22 @@
         <v>0</v>
       </c>
       <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
         <v>0.02</v>
       </c>
-      <c r="J74">
-        <v>0.5</v>
-      </c>
-      <c r="L74">
-        <v>23</v>
+      <c r="K74">
+        <v>0.5</v>
       </c>
       <c r="M74">
         <v>23</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N74">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>39</v>
       </c>
@@ -6503,19 +6728,22 @@
         <v>0</v>
       </c>
       <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
         <v>0.02</v>
       </c>
-      <c r="J75">
-        <v>0.5</v>
-      </c>
-      <c r="L75">
-        <v>23</v>
+      <c r="K75">
+        <v>0.5</v>
       </c>
       <c r="M75">
         <v>23</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>40</v>
       </c>
@@ -6541,19 +6769,22 @@
         <v>0</v>
       </c>
       <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
         <v>0.02</v>
       </c>
-      <c r="J76">
-        <v>0.5</v>
-      </c>
-      <c r="L76">
-        <v>23</v>
+      <c r="K76">
+        <v>0.5</v>
       </c>
       <c r="M76">
         <v>23</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N76">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>41</v>
       </c>
@@ -6579,19 +6810,22 @@
         <v>0</v>
       </c>
       <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
         <v>0.02</v>
       </c>
-      <c r="J77">
-        <v>0.5</v>
-      </c>
-      <c r="L77">
-        <v>23</v>
+      <c r="K77">
+        <v>0.5</v>
       </c>
       <c r="M77">
         <v>23</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N77">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>42</v>
       </c>
@@ -6617,19 +6851,22 @@
         <v>0</v>
       </c>
       <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
         <v>0.02</v>
       </c>
-      <c r="J78">
-        <v>0.5</v>
-      </c>
-      <c r="L78">
-        <v>28</v>
+      <c r="K78">
+        <v>0.5</v>
       </c>
       <c r="M78">
         <v>28</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N78">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>43</v>
       </c>
@@ -6655,19 +6892,22 @@
         <v>0</v>
       </c>
       <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
         <v>0.02</v>
       </c>
-      <c r="J79">
-        <v>0.5</v>
-      </c>
-      <c r="L79">
-        <v>28</v>
+      <c r="K79">
+        <v>0.5</v>
       </c>
       <c r="M79">
         <v>28</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N79">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>44</v>
       </c>
@@ -6693,19 +6933,22 @@
         <v>0</v>
       </c>
       <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
         <v>0.02</v>
       </c>
-      <c r="J80">
-        <v>0.5</v>
-      </c>
-      <c r="L80">
-        <v>23</v>
+      <c r="K80">
+        <v>0.5</v>
       </c>
       <c r="M80">
         <v>23</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N80">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>45</v>
       </c>
@@ -6731,15 +6974,18 @@
         <v>0</v>
       </c>
       <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
         <v>0.02</v>
       </c>
-      <c r="J81">
-        <v>0.5</v>
-      </c>
-      <c r="L81">
+      <c r="K81">
+        <v>0.5</v>
+      </c>
+      <c r="M81">
         <v>23</v>
       </c>
-      <c r="M81">
+      <c r="N81">
         <v>23</v>
       </c>
     </row>
@@ -7778,7 +8024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>

</xml_diff>